<commit_message>
include some feedback. Thanks to shartqueefa (shmups forum user) for that :)
</commit_message>
<xml_diff>
--- a/RGB Bypass/BOM_SNES_RGB_bypass.xlsx
+++ b/RGB Bypass/BOM_SNES_RGB_bypass.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28908"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UserData\Bartmann\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/ToshibaHDWM110/borti4938/Documents/Workspaces/GitHub/SNES-AddOn-PCBs/RGB Bypass/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="25605" windowHeight="14445" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14440"/>
   </bookViews>
   <sheets>
     <sheet name="SNES_RGBAmp" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="96">
   <si>
     <t>Designator</t>
   </si>
@@ -139,12 +139,6 @@
     <t>R12,R22,R32</t>
   </si>
   <si>
-    <t>CRCW06035M23FKEA</t>
-  </si>
-  <si>
-    <t>5.2MOhm, 0.1W</t>
-  </si>
-  <si>
     <t>R13,R23,R33</t>
   </si>
   <si>
@@ -169,9 +163,6 @@
     <t>Decoupling caps on modding board</t>
   </si>
   <si>
-    <t>CBR06C470JAGAC</t>
-  </si>
-  <si>
     <t>Ceramic capacitor, C0G/NP0</t>
   </si>
   <si>
@@ -241,9 +232,6 @@
     <t>R43</t>
   </si>
   <si>
-    <t>47pF +/-5% / 250V</t>
-  </si>
-  <si>
     <t>Short</t>
   </si>
   <si>
@@ -314,13 +302,28 @@
   </si>
   <si>
     <t>220uF +/- 10% / 6.3V</t>
+  </si>
+  <si>
+    <t>CRCW06035M10FKEA</t>
+  </si>
+  <si>
+    <t>5.1MOhm, 0.1W</t>
+  </si>
+  <si>
+    <t>CL10C470JB8NNNC</t>
+  </si>
+  <si>
+    <t>47pF +/-5% / 50V</t>
+  </si>
+  <si>
+    <t>7,30 mm x 4,30 mm, alternative to the 330uF tantalum capacitor</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="19" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -463,6 +466,29 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -761,7 +787,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="43">
+  <cellStyleXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -805,8 +831,10 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
@@ -819,6 +847,12 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -827,14 +861,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="43">
+  <cellStyles count="45">
     <cellStyle name="20 % - Akzent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20 % - Akzent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20 % - Akzent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -861,15 +894,17 @@
     <cellStyle name="Akzent6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="Ausgabe" xfId="10" builtinId="21" customBuiltin="1"/>
     <cellStyle name="Berechnung" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Besuchter Link" xfId="43" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="44" builtinId="9" hidden="1"/>
     <cellStyle name="Eingabe" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Ergebnis" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Erklärender Text" xfId="16" builtinId="53" customBuiltin="1"/>
     <cellStyle name="Gut" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Link" xfId="42" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="42" builtinId="8"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Notiz" xfId="15" builtinId="10" customBuiltin="1"/>
     <cellStyle name="Schlecht" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Stand." xfId="0" builtinId="0"/>
     <cellStyle name="Überschrift" xfId="1" builtinId="15" customBuiltin="1"/>
     <cellStyle name="Überschrift 1" xfId="2" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Überschrift 2" xfId="3" builtinId="17" customBuiltin="1"/>
@@ -1157,18 +1192,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I36"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="16.42578125" customWidth="1"/>
-    <col min="4" max="4" width="23.42578125" customWidth="1"/>
-    <col min="5" max="5" width="18.42578125" customWidth="1"/>
-    <col min="7" max="7" width="59.85546875" customWidth="1"/>
-    <col min="8" max="8" width="11.28515625" customWidth="1"/>
+    <col min="2" max="2" width="16.5" customWidth="1"/>
+    <col min="4" max="4" width="23.5" customWidth="1"/>
+    <col min="5" max="5" width="18.5" customWidth="1"/>
+    <col min="7" max="7" width="59.83203125" customWidth="1"/>
+    <col min="8" max="8" width="11.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -1191,7 +1226,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1210,7 +1245,7 @@
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>18</v>
       </c>
@@ -1226,7 +1261,7 @@
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>23</v>
       </c>
@@ -1242,7 +1277,7 @@
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>24</v>
       </c>
@@ -1258,7 +1293,7 @@
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>28</v>
       </c>
@@ -1280,7 +1315,7 @@
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>29</v>
       </c>
@@ -1302,31 +1337,31 @@
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="D8" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="E8" t="s">
+        <v>74</v>
+      </c>
+      <c r="F8" t="s">
+        <v>79</v>
+      </c>
+      <c r="G8" t="s">
         <v>78</v>
-      </c>
-      <c r="F8" t="s">
-        <v>83</v>
-      </c>
-      <c r="G8" t="s">
-        <v>82</v>
       </c>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C9">
         <v>1</v>
@@ -1335,18 +1370,18 @@
         <v>15</v>
       </c>
       <c r="E9" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="F9" t="s">
         <v>14</v>
       </c>
       <c r="G9" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>32</v>
       </c>
@@ -1368,12 +1403,12 @@
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>35</v>
       </c>
       <c r="B11" t="s">
-        <v>36</v>
+        <v>91</v>
       </c>
       <c r="C11">
         <v>3</v>
@@ -1382,7 +1417,7 @@
         <v>15</v>
       </c>
       <c r="E11" t="s">
-        <v>37</v>
+        <v>92</v>
       </c>
       <c r="F11" t="s">
         <v>14</v>
@@ -1390,9 +1425,9 @@
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B12" t="s">
         <v>16</v>
@@ -1404,192 +1439,192 @@
         <v>15</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F12" t="s">
         <v>14</v>
       </c>
       <c r="G12" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D13" t="s">
         <v>15</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F13" t="s">
         <v>14</v>
       </c>
       <c r="G13" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
+        <v>41</v>
+      </c>
+      <c r="B15" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="C15" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="D15" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="E15" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="F15" t="s">
+        <v>14</v>
+      </c>
+      <c r="G15" s="7" t="s">
         <v>43</v>
-      </c>
-      <c r="B15" t="s">
-        <v>46</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="D15" t="s">
-        <v>47</v>
-      </c>
-      <c r="E15" t="s">
-        <v>70</v>
-      </c>
-      <c r="F15" t="s">
-        <v>14</v>
-      </c>
-      <c r="G15" s="7" t="s">
-        <v>45</v>
       </c>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C16" s="6"/>
       <c r="G16" s="7"/>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="9" t="s">
-        <v>50</v>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A17" s="11" t="s">
+        <v>47</v>
       </c>
       <c r="B17" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C17" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="D17" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E17" t="s">
+        <v>49</v>
+      </c>
+      <c r="F17" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="G17" s="9" t="s">
         <v>51</v>
-      </c>
-      <c r="C17" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="D17" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="E17" t="s">
-        <v>52</v>
-      </c>
-      <c r="F17" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="G17" s="11" t="s">
-        <v>54</v>
       </c>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="9"/>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A18" s="11"/>
       <c r="B18" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="C18" s="10"/>
-      <c r="D18" s="9"/>
+        <v>46</v>
+      </c>
+      <c r="C18" s="12"/>
+      <c r="D18" s="11"/>
       <c r="E18" t="s">
-        <v>53</v>
-      </c>
-      <c r="F18" s="12"/>
-      <c r="G18" s="11" t="s">
-        <v>55</v>
+        <v>50</v>
+      </c>
+      <c r="F18" s="13"/>
+      <c r="G18" s="9" t="s">
+        <v>52</v>
       </c>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="B22" s="8"/>
-      <c r="C22" s="8"/>
-      <c r="D22" s="8"/>
-      <c r="E22" s="8"/>
-      <c r="F22" s="8"/>
-      <c r="G22" s="8"/>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A22" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="B22" s="10"/>
+      <c r="C22" s="10"/>
+      <c r="D22" s="10"/>
+      <c r="E22" s="10"/>
+      <c r="F22" s="10"/>
+      <c r="G22" s="10"/>
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B24" s="2"/>
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B26" s="2"/>
       <c r="E26" s="3"/>
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B27" s="2"/>
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="E28" s="3"/>
       <c r="H28" s="1"/>
       <c r="I28" s="1"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="E30" s="3"/>
       <c r="H30" s="1"/>
       <c r="I30" s="1"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="E31" s="3"/>
       <c r="G31" s="2"/>
       <c r="H31" s="4"/>
       <c r="I31" s="5"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="E32" s="3"/>
       <c r="G32" s="2"/>
       <c r="H32" s="4"/>
       <c r="I32" s="1"/>
     </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B35" s="1"/>
     </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B36" s="1"/>
     </row>
   </sheetData>
@@ -1607,20 +1642,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I47"/>
+  <dimension ref="A1:I48"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="16.42578125" customWidth="1"/>
-    <col min="4" max="4" width="23.42578125" customWidth="1"/>
-    <col min="5" max="5" width="18.42578125" customWidth="1"/>
-    <col min="7" max="7" width="59.85546875" customWidth="1"/>
-    <col min="8" max="8" width="11.28515625" customWidth="1"/>
+    <col min="2" max="2" width="16.5" customWidth="1"/>
+    <col min="4" max="4" width="23.5" customWidth="1"/>
+    <col min="5" max="5" width="18.5" customWidth="1"/>
+    <col min="7" max="7" width="59.83203125" customWidth="1"/>
+    <col min="8" max="8" width="11.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -1643,7 +1678,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1662,7 +1697,7 @@
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>18</v>
       </c>
@@ -1678,7 +1713,7 @@
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>28</v>
       </c>
@@ -1700,7 +1735,7 @@
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>29</v>
       </c>
@@ -1722,31 +1757,31 @@
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="D6" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="E6" t="s">
+        <v>74</v>
+      </c>
+      <c r="F6" t="s">
+        <v>79</v>
+      </c>
+      <c r="G6" t="s">
         <v>78</v>
-      </c>
-      <c r="F6" t="s">
-        <v>83</v>
-      </c>
-      <c r="G6" t="s">
-        <v>82</v>
       </c>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -1755,18 +1790,18 @@
         <v>15</v>
       </c>
       <c r="E7" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="F7" t="s">
         <v>14</v>
       </c>
       <c r="G7" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>32</v>
       </c>
@@ -1788,12 +1823,12 @@
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>35</v>
       </c>
       <c r="B9" t="s">
-        <v>36</v>
+        <v>91</v>
       </c>
       <c r="C9">
         <v>3</v>
@@ -1802,7 +1837,7 @@
         <v>15</v>
       </c>
       <c r="E9" t="s">
-        <v>37</v>
+        <v>92</v>
       </c>
       <c r="F9" t="s">
         <v>14</v>
@@ -1810,9 +1845,9 @@
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B10" t="s">
         <v>16</v>
@@ -1824,130 +1859,130 @@
         <v>15</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F10" t="s">
         <v>14</v>
       </c>
       <c r="G10" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D11" t="s">
         <v>15</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F11" t="s">
         <v>14</v>
       </c>
       <c r="G11" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
+        <v>41</v>
+      </c>
+      <c r="B13" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="C13" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="D13" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="E13" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="F13" t="s">
+        <v>14</v>
+      </c>
+      <c r="G13" s="7" t="s">
         <v>43</v>
-      </c>
-      <c r="B13" t="s">
-        <v>46</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="D13" t="s">
-        <v>47</v>
-      </c>
-      <c r="E13" t="s">
-        <v>70</v>
-      </c>
-      <c r="F13" t="s">
-        <v>14</v>
-      </c>
-      <c r="G13" s="7" t="s">
-        <v>45</v>
       </c>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C14" s="6"/>
       <c r="G14" s="7"/>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="9" t="s">
-        <v>50</v>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A15" s="11" t="s">
+        <v>47</v>
       </c>
       <c r="B15" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C15" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="D15" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="E15" t="s">
+        <v>49</v>
+      </c>
+      <c r="F15" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="G15" s="9" t="s">
         <v>51</v>
-      </c>
-      <c r="C15" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="D15" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="E15" t="s">
-        <v>52</v>
-      </c>
-      <c r="F15" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="G15" s="11" t="s">
-        <v>54</v>
       </c>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="9"/>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A16" s="11"/>
       <c r="B16" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="C16" s="13"/>
-      <c r="D16" s="12"/>
+        <v>46</v>
+      </c>
+      <c r="C16" s="14"/>
+      <c r="D16" s="13"/>
       <c r="E16" t="s">
-        <v>53</v>
-      </c>
-      <c r="F16" s="12"/>
-      <c r="G16" s="11" t="s">
-        <v>55</v>
+        <v>50</v>
+      </c>
+      <c r="F16" s="13"/>
+      <c r="G16" s="9" t="s">
+        <v>52</v>
       </c>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="6" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C19">
         <v>1</v>
@@ -1956,7 +1991,7 @@
         <v>15</v>
       </c>
       <c r="E19" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="F19" t="s">
         <v>14</v>
@@ -1964,12 +1999,12 @@
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="7" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B20" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C20">
         <v>1</v>
@@ -1978,7 +2013,7 @@
         <v>15</v>
       </c>
       <c r="E20" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="F20" t="s">
         <v>14</v>
@@ -1986,117 +2021,118 @@
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="7" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B21" t="s">
+        <v>71</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+      <c r="D21" t="s">
+        <v>72</v>
+      </c>
+      <c r="E21" t="s">
         <v>75</v>
       </c>
-      <c r="C21">
-        <v>1</v>
-      </c>
-      <c r="D21" t="s">
+      <c r="F21" t="s">
+        <v>77</v>
+      </c>
+      <c r="G21" t="s">
         <v>76</v>
-      </c>
-      <c r="E21" t="s">
-        <v>79</v>
-      </c>
-      <c r="F21" t="s">
-        <v>81</v>
-      </c>
-      <c r="G21" t="s">
-        <v>80</v>
       </c>
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="7" t="s">
-        <v>69</v>
-      </c>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A22" s="7"/>
       <c r="B22" t="s">
-        <v>16</v>
+        <v>89</v>
       </c>
       <c r="C22">
         <v>1</v>
       </c>
       <c r="D22" t="s">
-        <v>15</v>
-      </c>
-      <c r="E22" s="3" t="s">
-        <v>39</v>
+        <v>72</v>
+      </c>
+      <c r="E22" t="s">
+        <v>90</v>
       </c>
       <c r="F22" t="s">
-        <v>14</v>
+        <v>77</v>
+      </c>
+      <c r="G22" t="s">
+        <v>95</v>
       </c>
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="7" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="B23" t="s">
-        <v>46</v>
-      </c>
-      <c r="C23" s="6" t="s">
-        <v>44</v>
+        <v>16</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
       </c>
       <c r="D23" t="s">
-        <v>47</v>
-      </c>
-      <c r="E23" t="s">
-        <v>70</v>
+        <v>15</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>37</v>
       </c>
       <c r="F23" t="s">
         <v>14</v>
-      </c>
-      <c r="G23" s="7" t="s">
-        <v>45</v>
       </c>
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A24" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="B24" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="C24" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="D24" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="E24" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="F24" t="s">
+        <v>14</v>
+      </c>
+      <c r="G24" s="7" t="s">
+        <v>43</v>
+      </c>
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="6" t="s">
-        <v>85</v>
-      </c>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="C26">
-        <v>1</v>
-      </c>
-      <c r="D26" t="s">
-        <v>15</v>
-      </c>
-      <c r="E26" t="s">
-        <v>59</v>
-      </c>
-      <c r="F26" t="s">
-        <v>14</v>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A26" s="6" t="s">
+        <v>81</v>
       </c>
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="B27" t="s">
-        <v>66</v>
+        <v>54</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>61</v>
       </c>
       <c r="C27">
         <v>1</v>
@@ -2105,7 +2141,7 @@
         <v>15</v>
       </c>
       <c r="E27" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="F27" t="s">
         <v>14</v>
@@ -2113,147 +2149,169 @@
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="G28" t="s">
-        <v>74</v>
+        <v>57</v>
+      </c>
+      <c r="B28" t="s">
+        <v>63</v>
+      </c>
+      <c r="C28">
+        <v>1</v>
+      </c>
+      <c r="D28" t="s">
+        <v>15</v>
+      </c>
+      <c r="E28" t="s">
+        <v>64</v>
+      </c>
+      <c r="F28" t="s">
+        <v>14</v>
       </c>
       <c r="H28" s="1"/>
       <c r="I28" s="1"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="B29" t="s">
-        <v>16</v>
-      </c>
-      <c r="C29">
-        <v>1</v>
-      </c>
-      <c r="D29" t="s">
-        <v>15</v>
-      </c>
-      <c r="E29" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="F29" t="s">
-        <v>14</v>
+        <v>65</v>
+      </c>
+      <c r="G29" t="s">
+        <v>70</v>
       </c>
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="7"/>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A30" s="7" t="s">
+        <v>66</v>
+      </c>
       <c r="B30" t="s">
-        <v>71</v>
-      </c>
-      <c r="G30" t="s">
-        <v>72</v>
+        <v>16</v>
+      </c>
+      <c r="C30">
+        <v>1</v>
+      </c>
+      <c r="D30" t="s">
+        <v>15</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="F30" t="s">
+        <v>14</v>
       </c>
       <c r="H30" s="1"/>
       <c r="I30" s="1"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" s="7" t="s">
-        <v>73</v>
-      </c>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A31" s="7"/>
       <c r="B31" t="s">
-        <v>46</v>
-      </c>
-      <c r="C31" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="D31" t="s">
-        <v>47</v>
-      </c>
-      <c r="E31" t="s">
-        <v>70</v>
-      </c>
-      <c r="F31" t="s">
-        <v>14</v>
-      </c>
-      <c r="G31" s="7" t="s">
-        <v>45</v>
+        <v>67</v>
+      </c>
+      <c r="G31" t="s">
+        <v>68</v>
       </c>
       <c r="H31" s="1"/>
       <c r="I31" s="1"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" s="7"/>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A32" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="B32" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="C32" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="D32" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="E32" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="F32" t="s">
+        <v>14</v>
+      </c>
+      <c r="G32" s="7" t="s">
+        <v>43</v>
+      </c>
       <c r="H32" s="1"/>
       <c r="I32" s="1"/>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="B33" s="8"/>
-      <c r="C33" s="8"/>
-      <c r="D33" s="8"/>
-      <c r="E33" s="8"/>
-      <c r="F33" s="8"/>
-      <c r="G33" s="8"/>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A33" s="7"/>
       <c r="H33" s="1"/>
       <c r="I33" s="1"/>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A34" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="B34" s="10"/>
+      <c r="C34" s="10"/>
+      <c r="D34" s="10"/>
+      <c r="E34" s="10"/>
+      <c r="F34" s="10"/>
+      <c r="G34" s="10"/>
       <c r="H34" s="1"/>
       <c r="I34" s="1"/>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B35" s="2"/>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="H35" s="1"/>
       <c r="I35" s="1"/>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B36" s="2"/>
       <c r="H36" s="1"/>
       <c r="I36" s="1"/>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B37" s="2"/>
-      <c r="E37" s="3"/>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="H37" s="1"/>
       <c r="I37" s="1"/>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B38" s="2"/>
+      <c r="E38" s="3"/>
       <c r="H38" s="1"/>
       <c r="I38" s="1"/>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E39" s="3"/>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B39" s="2"/>
       <c r="H39" s="1"/>
       <c r="I39" s="1"/>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="E40" s="3"/>
       <c r="H40" s="1"/>
       <c r="I40" s="1"/>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E41" s="3"/>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="H41" s="1"/>
       <c r="I41" s="1"/>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="E42" s="3"/>
-      <c r="G42" s="2"/>
-      <c r="H42" s="4"/>
-      <c r="I42" s="5"/>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H42" s="1"/>
+      <c r="I42" s="1"/>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="E43" s="3"/>
       <c r="G43" s="2"/>
       <c r="H43" s="4"/>
-      <c r="I43" s="1"/>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B46" s="1"/>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I43" s="5"/>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="E44" s="3"/>
+      <c r="G44" s="2"/>
+      <c r="H44" s="4"/>
+      <c r="I44" s="1"/>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B47" s="1"/>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B48" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -2261,7 +2319,7 @@
     <mergeCell ref="C15:C16"/>
     <mergeCell ref="D15:D16"/>
     <mergeCell ref="F15:F16"/>
-    <mergeCell ref="A33:G33"/>
+    <mergeCell ref="A34:G34"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
@@ -2270,20 +2328,20 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I55"/>
+  <dimension ref="A1:I56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="16.42578125" customWidth="1"/>
-    <col min="4" max="4" width="23.42578125" customWidth="1"/>
-    <col min="5" max="5" width="18.42578125" customWidth="1"/>
-    <col min="7" max="7" width="59.85546875" customWidth="1"/>
-    <col min="8" max="8" width="11.28515625" customWidth="1"/>
+    <col min="2" max="2" width="16.5" customWidth="1"/>
+    <col min="4" max="4" width="23.5" customWidth="1"/>
+    <col min="5" max="5" width="18.5" customWidth="1"/>
+    <col min="7" max="7" width="59.83203125" customWidth="1"/>
+    <col min="8" max="8" width="11.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -2306,7 +2364,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -2325,7 +2383,7 @@
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>18</v>
       </c>
@@ -2341,7 +2399,7 @@
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>28</v>
       </c>
@@ -2363,7 +2421,7 @@
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>29</v>
       </c>
@@ -2385,31 +2443,31 @@
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="D6" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="E6" t="s">
+        <v>74</v>
+      </c>
+      <c r="F6" t="s">
+        <v>79</v>
+      </c>
+      <c r="G6" t="s">
         <v>78</v>
-      </c>
-      <c r="F6" t="s">
-        <v>83</v>
-      </c>
-      <c r="G6" t="s">
-        <v>82</v>
       </c>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -2418,18 +2476,18 @@
         <v>15</v>
       </c>
       <c r="E7" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="F7" t="s">
         <v>14</v>
       </c>
       <c r="G7" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>32</v>
       </c>
@@ -2451,12 +2509,12 @@
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>35</v>
       </c>
       <c r="B9" t="s">
-        <v>36</v>
+        <v>91</v>
       </c>
       <c r="C9">
         <v>3</v>
@@ -2465,7 +2523,7 @@
         <v>15</v>
       </c>
       <c r="E9" t="s">
-        <v>37</v>
+        <v>92</v>
       </c>
       <c r="F9" t="s">
         <v>14</v>
@@ -2473,9 +2531,9 @@
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B10" t="s">
         <v>16</v>
@@ -2487,130 +2545,130 @@
         <v>15</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F10" t="s">
         <v>14</v>
       </c>
       <c r="G10" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D11" t="s">
         <v>15</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F11" t="s">
         <v>14</v>
       </c>
       <c r="G11" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
+        <v>41</v>
+      </c>
+      <c r="B13" t="s">
+        <v>93</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="D13" t="s">
+        <v>44</v>
+      </c>
+      <c r="E13" t="s">
+        <v>94</v>
+      </c>
+      <c r="F13" t="s">
+        <v>14</v>
+      </c>
+      <c r="G13" s="7" t="s">
         <v>43</v>
-      </c>
-      <c r="B13" t="s">
-        <v>46</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="D13" t="s">
-        <v>47</v>
-      </c>
-      <c r="E13" t="s">
-        <v>70</v>
-      </c>
-      <c r="F13" t="s">
-        <v>14</v>
-      </c>
-      <c r="G13" s="7" t="s">
-        <v>45</v>
       </c>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C14" s="6"/>
       <c r="G14" s="7"/>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="9" t="s">
-        <v>50</v>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A15" s="11" t="s">
+        <v>47</v>
       </c>
       <c r="B15" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C15" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="D15" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="E15" t="s">
+        <v>49</v>
+      </c>
+      <c r="F15" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="G15" s="9" t="s">
         <v>51</v>
-      </c>
-      <c r="C15" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="D15" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="E15" t="s">
-        <v>52</v>
-      </c>
-      <c r="F15" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="G15" s="11" t="s">
-        <v>54</v>
       </c>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="9"/>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A16" s="11"/>
       <c r="B16" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="C16" s="13"/>
-      <c r="D16" s="12"/>
+        <v>46</v>
+      </c>
+      <c r="C16" s="14"/>
+      <c r="D16" s="13"/>
       <c r="E16" t="s">
-        <v>53</v>
-      </c>
-      <c r="F16" s="12"/>
-      <c r="G16" s="11" t="s">
-        <v>55</v>
+        <v>50</v>
+      </c>
+      <c r="F16" s="13"/>
+      <c r="G16" s="9" t="s">
+        <v>52</v>
       </c>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="6" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C19">
         <v>1</v>
@@ -2619,7 +2677,7 @@
         <v>15</v>
       </c>
       <c r="E19" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="F19" t="s">
         <v>14</v>
@@ -2627,12 +2685,12 @@
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="7" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B20" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C20">
         <v>1</v>
@@ -2641,7 +2699,7 @@
         <v>15</v>
       </c>
       <c r="E20" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="F20" t="s">
         <v>14</v>
@@ -2649,117 +2707,117 @@
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="7" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B21" t="s">
+        <v>71</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+      <c r="D21" t="s">
+        <v>72</v>
+      </c>
+      <c r="E21" t="s">
         <v>75</v>
       </c>
-      <c r="C21">
-        <v>1</v>
-      </c>
-      <c r="D21" t="s">
+      <c r="F21" t="s">
+        <v>77</v>
+      </c>
+      <c r="G21" t="s">
         <v>76</v>
-      </c>
-      <c r="E21" t="s">
-        <v>79</v>
-      </c>
-      <c r="F21" t="s">
-        <v>81</v>
-      </c>
-      <c r="G21" t="s">
-        <v>80</v>
       </c>
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="7" t="s">
-        <v>69</v>
-      </c>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
-        <v>16</v>
+        <v>89</v>
       </c>
       <c r="C22">
         <v>1</v>
       </c>
       <c r="D22" t="s">
-        <v>15</v>
-      </c>
-      <c r="E22" s="3" t="s">
-        <v>39</v>
+        <v>72</v>
+      </c>
+      <c r="E22" t="s">
+        <v>90</v>
       </c>
       <c r="F22" t="s">
-        <v>14</v>
+        <v>77</v>
+      </c>
+      <c r="G22" t="s">
+        <v>95</v>
       </c>
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="7" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="B23" t="s">
-        <v>46</v>
-      </c>
-      <c r="C23" s="6" t="s">
-        <v>44</v>
+        <v>16</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
       </c>
       <c r="D23" t="s">
-        <v>47</v>
-      </c>
-      <c r="E23" t="s">
-        <v>70</v>
+        <v>15</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>37</v>
       </c>
       <c r="F23" t="s">
         <v>14</v>
       </c>
       <c r="G23" s="7" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A24" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="B24" t="s">
+        <v>93</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="D24" t="s">
+        <v>44</v>
+      </c>
+      <c r="E24" t="s">
+        <v>94</v>
+      </c>
+      <c r="F24" t="s">
+        <v>14</v>
+      </c>
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="6" t="s">
-        <v>85</v>
-      </c>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="C26">
-        <v>1</v>
-      </c>
-      <c r="D26" t="s">
-        <v>15</v>
-      </c>
-      <c r="E26" t="s">
-        <v>59</v>
-      </c>
-      <c r="F26" t="s">
-        <v>14</v>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A26" s="6" t="s">
+        <v>81</v>
       </c>
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="B27" t="s">
-        <v>66</v>
+        <v>54</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>61</v>
       </c>
       <c r="C27">
         <v>1</v>
@@ -2768,7 +2826,7 @@
         <v>15</v>
       </c>
       <c r="E27" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="F27" t="s">
         <v>14</v>
@@ -2776,307 +2834,326 @@
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" s="7" t="s">
-        <v>68</v>
+        <v>57</v>
+      </c>
+      <c r="B28" t="s">
+        <v>63</v>
+      </c>
+      <c r="C28">
+        <v>1</v>
+      </c>
+      <c r="D28" t="s">
+        <v>15</v>
+      </c>
+      <c r="E28" t="s">
+        <v>64</v>
+      </c>
+      <c r="F28" t="s">
+        <v>14</v>
       </c>
       <c r="G28" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="H28" s="1"/>
       <c r="I28" s="1"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="B29" t="s">
-        <v>16</v>
-      </c>
-      <c r="C29">
-        <v>1</v>
-      </c>
-      <c r="D29" t="s">
-        <v>15</v>
-      </c>
-      <c r="E29" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="F29" t="s">
-        <v>14</v>
+        <v>65</v>
       </c>
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="7"/>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A30" s="7" t="s">
+        <v>66</v>
+      </c>
       <c r="B30" t="s">
-        <v>71</v>
+        <v>16</v>
+      </c>
+      <c r="C30">
+        <v>1</v>
+      </c>
+      <c r="D30" t="s">
+        <v>15</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="F30" t="s">
+        <v>14</v>
       </c>
       <c r="G30" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="H30" s="1"/>
       <c r="I30" s="1"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" s="7" t="s">
-        <v>73</v>
-      </c>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A31" s="7"/>
       <c r="B31" t="s">
-        <v>46</v>
-      </c>
-      <c r="C31" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="D31" t="s">
-        <v>47</v>
-      </c>
-      <c r="E31" t="s">
-        <v>70</v>
-      </c>
-      <c r="F31" t="s">
-        <v>14</v>
+        <v>67</v>
       </c>
       <c r="G31" s="7" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="H31" s="1"/>
       <c r="I31" s="1"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" s="7"/>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A32" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="B32" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="C32" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="D32" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="E32" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="F32" t="s">
+        <v>14</v>
+      </c>
       <c r="H32" s="1"/>
       <c r="I32" s="1"/>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" s="6" t="s">
-        <v>86</v>
-      </c>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A33" s="7"/>
       <c r="H33" s="1"/>
       <c r="I33" s="1"/>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34" s="7" t="s">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A34" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="G34" t="s">
         <v>87</v>
-      </c>
-      <c r="B34" t="s">
-        <v>16</v>
-      </c>
-      <c r="C34">
-        <v>2</v>
-      </c>
-      <c r="D34" t="s">
-        <v>15</v>
-      </c>
-      <c r="E34" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="F34" t="s">
-        <v>14</v>
-      </c>
-      <c r="G34" t="s">
-        <v>91</v>
       </c>
       <c r="H34" s="1"/>
       <c r="I34" s="1"/>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35" s="6"/>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A35" s="7" t="s">
+        <v>83</v>
+      </c>
       <c r="B35" t="s">
-        <v>40</v>
+        <v>16</v>
+      </c>
+      <c r="C35">
+        <v>2</v>
       </c>
       <c r="D35" t="s">
         <v>15</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="F35" t="s">
         <v>14</v>
       </c>
       <c r="G35" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H35" s="1"/>
       <c r="I35" s="1"/>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A36" s="7" t="s">
-        <v>88</v>
-      </c>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A36" s="6"/>
       <c r="B36" t="s">
-        <v>93</v>
-      </c>
-      <c r="C36">
-        <v>1</v>
+        <v>38</v>
       </c>
       <c r="D36" t="s">
+        <v>15</v>
+      </c>
+      <c r="E36" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="F36" t="s">
+        <v>14</v>
+      </c>
+      <c r="G36" t="s">
         <v>76</v>
-      </c>
-      <c r="E36" t="s">
-        <v>94</v>
-      </c>
-      <c r="F36" t="s">
-        <v>81</v>
-      </c>
-      <c r="G36" t="s">
-        <v>80</v>
       </c>
       <c r="H36" s="1"/>
       <c r="I36" s="1"/>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A37" s="7"/>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A37" s="7" t="s">
+        <v>84</v>
+      </c>
       <c r="B37" t="s">
-        <v>75</v>
+        <v>89</v>
       </c>
       <c r="C37">
         <v>1</v>
       </c>
       <c r="D37" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="E37" t="s">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="F37" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="G37" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="H37" s="1"/>
       <c r="I37" s="1"/>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A38" s="7" t="s">
-        <v>89</v>
-      </c>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A38" s="7"/>
       <c r="B38" t="s">
-        <v>3</v>
+        <v>71</v>
       </c>
       <c r="C38">
         <v>1</v>
       </c>
       <c r="D38" t="s">
-        <v>13</v>
+        <v>72</v>
       </c>
       <c r="E38" t="s">
-        <v>30</v>
+        <v>75</v>
       </c>
       <c r="F38" t="s">
-        <v>14</v>
+        <v>77</v>
       </c>
       <c r="H38" s="1"/>
       <c r="I38" s="1"/>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" s="7" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="B39" t="s">
-        <v>46</v>
-      </c>
-      <c r="C39" s="6" t="s">
-        <v>44</v>
+        <v>3</v>
+      </c>
+      <c r="C39">
+        <v>1</v>
       </c>
       <c r="D39" t="s">
-        <v>47</v>
+        <v>13</v>
       </c>
       <c r="E39" t="s">
-        <v>70</v>
+        <v>30</v>
       </c>
       <c r="F39" t="s">
         <v>14</v>
       </c>
       <c r="G39" s="7" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="H39" s="1"/>
       <c r="I39" s="1"/>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A40" s="7"/>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A40" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="B40" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="C40" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="D40" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="E40" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="F40" t="s">
+        <v>14</v>
+      </c>
       <c r="H40" s="1"/>
       <c r="I40" s="1"/>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A41" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="B41" s="8"/>
-      <c r="C41" s="8"/>
-      <c r="D41" s="8"/>
-      <c r="E41" s="8"/>
-      <c r="F41" s="8"/>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A41" s="7"/>
       <c r="G41" s="8"/>
       <c r="H41" s="1"/>
       <c r="I41" s="1"/>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A42" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="B42" s="8"/>
+      <c r="C42" s="8"/>
+      <c r="D42" s="8"/>
+      <c r="E42" s="8"/>
+      <c r="F42" s="8"/>
       <c r="H42" s="1"/>
       <c r="I42" s="1"/>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B43" s="2"/>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="H43" s="1"/>
       <c r="I43" s="1"/>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B44" s="2"/>
       <c r="H44" s="1"/>
       <c r="I44" s="1"/>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B45" s="2"/>
-      <c r="E45" s="3"/>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="H45" s="1"/>
       <c r="I45" s="1"/>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B46" s="2"/>
+      <c r="E46" s="3"/>
       <c r="H46" s="1"/>
       <c r="I46" s="1"/>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E47" s="3"/>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B47" s="2"/>
       <c r="H47" s="1"/>
       <c r="I47" s="1"/>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="E48" s="3"/>
       <c r="H48" s="1"/>
       <c r="I48" s="1"/>
     </row>
-    <row r="49" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="E49" s="3"/>
+    <row r="49" spans="2:9" x14ac:dyDescent="0.2">
       <c r="H49" s="1"/>
       <c r="I49" s="1"/>
     </row>
-    <row r="50" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:9" x14ac:dyDescent="0.2">
       <c r="E50" s="3"/>
       <c r="G50" s="2"/>
       <c r="H50" s="4"/>
       <c r="I50" s="5"/>
     </row>
-    <row r="51" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:9" x14ac:dyDescent="0.2">
       <c r="E51" s="3"/>
       <c r="G51" s="2"/>
       <c r="H51" s="4"/>
       <c r="I51" s="1"/>
     </row>
-    <row r="54" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B54" s="1"/>
-    </row>
-    <row r="55" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="E52" s="3"/>
+    </row>
+    <row r="55" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B55" s="1"/>
     </row>
+    <row r="56" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B56" s="1"/>
+    </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="4">
     <mergeCell ref="A15:A16"/>
     <mergeCell ref="C15:C16"/>
     <mergeCell ref="D15:D16"/>
     <mergeCell ref="F15:F16"/>
-    <mergeCell ref="A41:G41"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>

</xml_diff>

<commit_message>
revert a small copy n paste error
</commit_message>
<xml_diff>
--- a/RGB Bypass/BOM_SNES_RGB_bypass.xlsx
+++ b/RGB Bypass/BOM_SNES_RGB_bypass.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28908"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/ToshibaHDWM110/borti4938/Documents/Workspaces/GitHub/SNES-AddOn-PCBs/RGB Bypass/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UserData\Bartmann\Documents\Workspaces\Git\SNES-AddOn-PCBs\RGB Bypass\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14440"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="25605" windowHeight="14445"/>
   </bookViews>
   <sheets>
     <sheet name="SNES_RGBAmp" sheetId="1" r:id="rId1"/>
     <sheet name="SNES_RGBAmp_wCSYNC" sheetId="8" r:id="rId2"/>
     <sheet name="SNES_RGBAmp_wCSYNC_SVid" sheetId="9" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="150001" refMode="R1C1" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="330"/>
@@ -322,7 +322,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -849,6 +849,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -864,8 +866,6 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="45">
     <cellStyle name="20 % - Akzent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -894,17 +894,17 @@
     <cellStyle name="Akzent6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="Ausgabe" xfId="10" builtinId="21" customBuiltin="1"/>
     <cellStyle name="Berechnung" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Besuchter Link" xfId="43" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="43" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="44" builtinId="9" hidden="1"/>
     <cellStyle name="Eingabe" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Ergebnis" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Erklärender Text" xfId="16" builtinId="53" customBuiltin="1"/>
     <cellStyle name="Gut" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Hyperlink" xfId="42" builtinId="8"/>
+    <cellStyle name="Link" xfId="42" builtinId="8"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Notiz" xfId="15" builtinId="10" customBuiltin="1"/>
     <cellStyle name="Schlecht" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Stand." xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
     <cellStyle name="Überschrift" xfId="1" builtinId="15" customBuiltin="1"/>
     <cellStyle name="Überschrift 1" xfId="2" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Überschrift 2" xfId="3" builtinId="17" customBuiltin="1"/>
@@ -1194,16 +1194,16 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="16.5" customWidth="1"/>
-    <col min="4" max="4" width="23.5" customWidth="1"/>
-    <col min="5" max="5" width="18.5" customWidth="1"/>
-    <col min="7" max="7" width="59.83203125" customWidth="1"/>
-    <col min="8" max="8" width="11.33203125" customWidth="1"/>
+    <col min="2" max="2" width="16.42578125" customWidth="1"/>
+    <col min="4" max="4" width="23.42578125" customWidth="1"/>
+    <col min="5" max="5" width="18.42578125" customWidth="1"/>
+    <col min="7" max="7" width="59.85546875" customWidth="1"/>
+    <col min="8" max="8" width="11.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -1226,7 +1226,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1245,7 +1245,7 @@
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>18</v>
       </c>
@@ -1261,7 +1261,7 @@
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>23</v>
       </c>
@@ -1277,7 +1277,7 @@
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>24</v>
       </c>
@@ -1293,7 +1293,7 @@
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>28</v>
       </c>
@@ -1315,7 +1315,7 @@
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>29</v>
       </c>
@@ -1337,7 +1337,7 @@
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>73</v>
       </c>
@@ -1356,7 +1356,7 @@
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>53</v>
       </c>
@@ -1381,7 +1381,7 @@
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>32</v>
       </c>
@@ -1403,7 +1403,7 @@
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>35</v>
       </c>
@@ -1425,7 +1425,7 @@
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>36</v>
       </c>
@@ -1450,7 +1450,7 @@
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>38</v>
       </c>
@@ -1469,24 +1469,24 @@
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>41</v>
       </c>
-      <c r="B15" s="15" t="s">
+      <c r="B15" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="C15" s="16" t="s">
+      <c r="C15" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="D15" s="15" t="s">
+      <c r="D15" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="E15" s="15" t="s">
+      <c r="E15" s="10" t="s">
         <v>94</v>
       </c>
       <c r="F15" t="s">
@@ -1498,29 +1498,29 @@
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C16" s="6"/>
       <c r="G16" s="7"/>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A17" s="11" t="s">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="13" t="s">
         <v>47</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="C17" s="12" t="s">
+      <c r="C17" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="D17" s="11" t="s">
+      <c r="D17" s="13" t="s">
         <v>15</v>
       </c>
       <c r="E17" t="s">
         <v>49</v>
       </c>
-      <c r="F17" s="13" t="s">
+      <c r="F17" s="15" t="s">
         <v>14</v>
       </c>
       <c r="G17" s="9" t="s">
@@ -1529,102 +1529,102 @@
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A18" s="11"/>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="13"/>
       <c r="B18" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C18" s="12"/>
-      <c r="D18" s="11"/>
+      <c r="C18" s="14"/>
+      <c r="D18" s="13"/>
       <c r="E18" t="s">
         <v>50</v>
       </c>
-      <c r="F18" s="13"/>
+      <c r="F18" s="15"/>
       <c r="G18" s="9" t="s">
         <v>52</v>
       </c>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A22" s="10" t="s">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="B22" s="10"/>
-      <c r="C22" s="10"/>
-      <c r="D22" s="10"/>
-      <c r="E22" s="10"/>
-      <c r="F22" s="10"/>
-      <c r="G22" s="10"/>
+      <c r="B22" s="12"/>
+      <c r="C22" s="12"/>
+      <c r="D22" s="12"/>
+      <c r="E22" s="12"/>
+      <c r="F22" s="12"/>
+      <c r="G22" s="12"/>
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B24" s="2"/>
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B26" s="2"/>
       <c r="E26" s="3"/>
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B27" s="2"/>
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E28" s="3"/>
       <c r="H28" s="1"/>
       <c r="I28" s="1"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E30" s="3"/>
       <c r="H30" s="1"/>
       <c r="I30" s="1"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E31" s="3"/>
       <c r="G31" s="2"/>
       <c r="H31" s="4"/>
       <c r="I31" s="5"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E32" s="3"/>
       <c r="G32" s="2"/>
       <c r="H32" s="4"/>
       <c r="I32" s="1"/>
     </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B35" s="1"/>
     </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B36" s="1"/>
     </row>
   </sheetData>
@@ -1646,16 +1646,16 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="16.5" customWidth="1"/>
-    <col min="4" max="4" width="23.5" customWidth="1"/>
-    <col min="5" max="5" width="18.5" customWidth="1"/>
-    <col min="7" max="7" width="59.83203125" customWidth="1"/>
-    <col min="8" max="8" width="11.33203125" customWidth="1"/>
+    <col min="2" max="2" width="16.42578125" customWidth="1"/>
+    <col min="4" max="4" width="23.42578125" customWidth="1"/>
+    <col min="5" max="5" width="18.42578125" customWidth="1"/>
+    <col min="7" max="7" width="59.85546875" customWidth="1"/>
+    <col min="8" max="8" width="11.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -1678,7 +1678,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1697,7 +1697,7 @@
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>18</v>
       </c>
@@ -1713,7 +1713,7 @@
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>28</v>
       </c>
@@ -1735,7 +1735,7 @@
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>29</v>
       </c>
@@ -1757,7 +1757,7 @@
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>73</v>
       </c>
@@ -1776,7 +1776,7 @@
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>53</v>
       </c>
@@ -1801,7 +1801,7 @@
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>32</v>
       </c>
@@ -1823,7 +1823,7 @@
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>35</v>
       </c>
@@ -1845,7 +1845,7 @@
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>36</v>
       </c>
@@ -1870,7 +1870,7 @@
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>38</v>
       </c>
@@ -1889,24 +1889,24 @@
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>41</v>
       </c>
-      <c r="B13" s="15" t="s">
+      <c r="B13" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="C13" s="16" t="s">
+      <c r="C13" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="D13" s="15" t="s">
+      <c r="D13" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="E13" s="15" t="s">
+      <c r="E13" s="10" t="s">
         <v>94</v>
       </c>
       <c r="F13" t="s">
@@ -1918,29 +1918,29 @@
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C14" s="6"/>
       <c r="G14" s="7"/>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A15" s="11" t="s">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="13" t="s">
         <v>47</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="C15" s="14" t="s">
+      <c r="C15" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="D15" s="13" t="s">
+      <c r="D15" s="15" t="s">
         <v>15</v>
       </c>
       <c r="E15" t="s">
-        <v>49</v>
-      </c>
-      <c r="F15" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="F15" s="15" t="s">
         <v>14</v>
       </c>
       <c r="G15" s="9" t="s">
@@ -1949,35 +1949,35 @@
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A16" s="11"/>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="13"/>
       <c r="B16" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C16" s="14"/>
-      <c r="D16" s="13"/>
+      <c r="C16" s="16"/>
+      <c r="D16" s="15"/>
       <c r="E16" t="s">
-        <v>50</v>
-      </c>
-      <c r="F16" s="13"/>
+        <v>49</v>
+      </c>
+      <c r="F16" s="15"/>
       <c r="G16" s="9" t="s">
         <v>52</v>
       </c>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
         <v>80</v>
       </c>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>54</v>
       </c>
@@ -1999,7 +1999,7 @@
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>57</v>
       </c>
@@ -2021,7 +2021,7 @@
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
         <v>65</v>
       </c>
@@ -2046,7 +2046,7 @@
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="7"/>
       <c r="B22" t="s">
         <v>89</v>
@@ -2069,7 +2069,7 @@
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
         <v>66</v>
       </c>
@@ -2091,20 +2091,20 @@
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="B24" s="15" t="s">
+      <c r="B24" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="C24" s="16" t="s">
+      <c r="C24" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="D24" s="15" t="s">
+      <c r="D24" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="E24" s="15" t="s">
+      <c r="E24" s="10" t="s">
         <v>94</v>
       </c>
       <c r="F24" t="s">
@@ -2116,18 +2116,18 @@
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
         <v>81</v>
       </c>
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
         <v>54</v>
       </c>
@@ -2149,7 +2149,7 @@
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
         <v>57</v>
       </c>
@@ -2171,7 +2171,7 @@
       <c r="H28" s="1"/>
       <c r="I28" s="1"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="7" t="s">
         <v>65</v>
       </c>
@@ -2181,7 +2181,7 @@
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
         <v>66</v>
       </c>
@@ -2203,7 +2203,7 @@
       <c r="H30" s="1"/>
       <c r="I30" s="1"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="7"/>
       <c r="B31" t="s">
         <v>67</v>
@@ -2214,20 +2214,20 @@
       <c r="H31" s="1"/>
       <c r="I31" s="1"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="B32" s="15" t="s">
+      <c r="B32" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="C32" s="16" t="s">
+      <c r="C32" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="D32" s="15" t="s">
+      <c r="D32" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="E32" s="15" t="s">
+      <c r="E32" s="10" t="s">
         <v>94</v>
       </c>
       <c r="F32" t="s">
@@ -2239,78 +2239,78 @@
       <c r="H32" s="1"/>
       <c r="I32" s="1"/>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="7"/>
       <c r="H33" s="1"/>
       <c r="I33" s="1"/>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A34" s="10" t="s">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="B34" s="10"/>
-      <c r="C34" s="10"/>
-      <c r="D34" s="10"/>
-      <c r="E34" s="10"/>
-      <c r="F34" s="10"/>
-      <c r="G34" s="10"/>
+      <c r="B34" s="12"/>
+      <c r="C34" s="12"/>
+      <c r="D34" s="12"/>
+      <c r="E34" s="12"/>
+      <c r="F34" s="12"/>
+      <c r="G34" s="12"/>
       <c r="H34" s="1"/>
       <c r="I34" s="1"/>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="H35" s="1"/>
       <c r="I35" s="1"/>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B36" s="2"/>
       <c r="H36" s="1"/>
       <c r="I36" s="1"/>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="H37" s="1"/>
       <c r="I37" s="1"/>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B38" s="2"/>
       <c r="E38" s="3"/>
       <c r="H38" s="1"/>
       <c r="I38" s="1"/>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B39" s="2"/>
       <c r="H39" s="1"/>
       <c r="I39" s="1"/>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E40" s="3"/>
       <c r="H40" s="1"/>
       <c r="I40" s="1"/>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="H41" s="1"/>
       <c r="I41" s="1"/>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E42" s="3"/>
       <c r="H42" s="1"/>
       <c r="I42" s="1"/>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E43" s="3"/>
       <c r="G43" s="2"/>
       <c r="H43" s="4"/>
       <c r="I43" s="5"/>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E44" s="3"/>
       <c r="G44" s="2"/>
       <c r="H44" s="4"/>
       <c r="I44" s="1"/>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B47" s="1"/>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B48" s="1"/>
     </row>
   </sheetData>
@@ -2332,16 +2332,16 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="16.5" customWidth="1"/>
-    <col min="4" max="4" width="23.5" customWidth="1"/>
-    <col min="5" max="5" width="18.5" customWidth="1"/>
-    <col min="7" max="7" width="59.83203125" customWidth="1"/>
-    <col min="8" max="8" width="11.33203125" customWidth="1"/>
+    <col min="2" max="2" width="16.42578125" customWidth="1"/>
+    <col min="4" max="4" width="23.42578125" customWidth="1"/>
+    <col min="5" max="5" width="18.42578125" customWidth="1"/>
+    <col min="7" max="7" width="59.85546875" customWidth="1"/>
+    <col min="8" max="8" width="11.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -2364,7 +2364,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -2383,7 +2383,7 @@
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>18</v>
       </c>
@@ -2399,7 +2399,7 @@
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>28</v>
       </c>
@@ -2421,7 +2421,7 @@
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>29</v>
       </c>
@@ -2443,7 +2443,7 @@
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>73</v>
       </c>
@@ -2462,7 +2462,7 @@
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>53</v>
       </c>
@@ -2487,7 +2487,7 @@
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>32</v>
       </c>
@@ -2509,7 +2509,7 @@
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>35</v>
       </c>
@@ -2531,7 +2531,7 @@
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>36</v>
       </c>
@@ -2556,7 +2556,7 @@
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>38</v>
       </c>
@@ -2575,11 +2575,11 @@
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>41</v>
       </c>
@@ -2604,29 +2604,29 @@
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C14" s="6"/>
       <c r="G14" s="7"/>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A15" s="11" t="s">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="13" t="s">
         <v>47</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="C15" s="14" t="s">
+      <c r="C15" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="D15" s="13" t="s">
+      <c r="D15" s="15" t="s">
         <v>15</v>
       </c>
       <c r="E15" t="s">
-        <v>49</v>
-      </c>
-      <c r="F15" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="F15" s="15" t="s">
         <v>14</v>
       </c>
       <c r="G15" s="9" t="s">
@@ -2635,35 +2635,35 @@
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A16" s="11"/>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="13"/>
       <c r="B16" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C16" s="14"/>
-      <c r="D16" s="13"/>
+      <c r="C16" s="16"/>
+      <c r="D16" s="15"/>
       <c r="E16" t="s">
-        <v>50</v>
-      </c>
-      <c r="F16" s="13"/>
+        <v>49</v>
+      </c>
+      <c r="F16" s="15"/>
       <c r="G16" s="9" t="s">
         <v>52</v>
       </c>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
         <v>80</v>
       </c>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>54</v>
       </c>
@@ -2685,7 +2685,7 @@
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>57</v>
       </c>
@@ -2707,7 +2707,7 @@
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
         <v>65</v>
       </c>
@@ -2732,7 +2732,7 @@
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>89</v>
       </c>
@@ -2754,7 +2754,7 @@
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
         <v>66</v>
       </c>
@@ -2779,7 +2779,7 @@
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
         <v>69</v>
       </c>
@@ -2801,18 +2801,18 @@
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
         <v>81</v>
       </c>
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
         <v>54</v>
       </c>
@@ -2834,7 +2834,7 @@
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
         <v>57</v>
       </c>
@@ -2859,14 +2859,14 @@
       <c r="H28" s="1"/>
       <c r="I28" s="1"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="7" t="s">
         <v>65</v>
       </c>
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
         <v>66</v>
       </c>
@@ -2891,7 +2891,7 @@
       <c r="H30" s="1"/>
       <c r="I30" s="1"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="7"/>
       <c r="B31" t="s">
         <v>67</v>
@@ -2902,20 +2902,20 @@
       <c r="H31" s="1"/>
       <c r="I31" s="1"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="B32" s="15" t="s">
+      <c r="B32" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="C32" s="16" t="s">
+      <c r="C32" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="D32" s="15" t="s">
+      <c r="D32" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="E32" s="15" t="s">
+      <c r="E32" s="10" t="s">
         <v>94</v>
       </c>
       <c r="F32" t="s">
@@ -2924,12 +2924,12 @@
       <c r="H32" s="1"/>
       <c r="I32" s="1"/>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="7"/>
       <c r="H33" s="1"/>
       <c r="I33" s="1"/>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
         <v>82</v>
       </c>
@@ -2939,7 +2939,7 @@
       <c r="H34" s="1"/>
       <c r="I34" s="1"/>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="7" t="s">
         <v>83</v>
       </c>
@@ -2964,7 +2964,7 @@
       <c r="H35" s="1"/>
       <c r="I35" s="1"/>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="6"/>
       <c r="B36" t="s">
         <v>38</v>
@@ -2984,7 +2984,7 @@
       <c r="H36" s="1"/>
       <c r="I36" s="1"/>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="7" t="s">
         <v>84</v>
       </c>
@@ -3009,7 +3009,7 @@
       <c r="H37" s="1"/>
       <c r="I37" s="1"/>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="7"/>
       <c r="B38" t="s">
         <v>71</v>
@@ -3029,7 +3029,7 @@
       <c r="H38" s="1"/>
       <c r="I38" s="1"/>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="7" t="s">
         <v>85</v>
       </c>
@@ -3054,20 +3054,20 @@
       <c r="H39" s="1"/>
       <c r="I39" s="1"/>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="B40" s="15" t="s">
+      <c r="B40" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="C40" s="16" t="s">
+      <c r="C40" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="D40" s="15" t="s">
+      <c r="D40" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="E40" s="15" t="s">
+      <c r="E40" s="10" t="s">
         <v>94</v>
       </c>
       <c r="F40" t="s">
@@ -3076,13 +3076,13 @@
       <c r="H40" s="1"/>
       <c r="I40" s="1"/>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="7"/>
       <c r="G41" s="8"/>
       <c r="H41" s="1"/>
       <c r="I41" s="1"/>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="8" t="s">
         <v>45</v>
       </c>
@@ -3094,58 +3094,58 @@
       <c r="H42" s="1"/>
       <c r="I42" s="1"/>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="H43" s="1"/>
       <c r="I43" s="1"/>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B44" s="2"/>
       <c r="H44" s="1"/>
       <c r="I44" s="1"/>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="H45" s="1"/>
       <c r="I45" s="1"/>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B46" s="2"/>
       <c r="E46" s="3"/>
       <c r="H46" s="1"/>
       <c r="I46" s="1"/>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B47" s="2"/>
       <c r="H47" s="1"/>
       <c r="I47" s="1"/>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E48" s="3"/>
       <c r="H48" s="1"/>
       <c r="I48" s="1"/>
     </row>
-    <row r="49" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="49" spans="2:9" x14ac:dyDescent="0.25">
       <c r="H49" s="1"/>
       <c r="I49" s="1"/>
     </row>
-    <row r="50" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:9" x14ac:dyDescent="0.25">
       <c r="E50" s="3"/>
       <c r="G50" s="2"/>
       <c r="H50" s="4"/>
       <c r="I50" s="5"/>
     </row>
-    <row r="51" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="51" spans="2:9" x14ac:dyDescent="0.25">
       <c r="E51" s="3"/>
       <c r="G51" s="2"/>
       <c r="H51" s="4"/>
       <c r="I51" s="1"/>
     </row>
-    <row r="52" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="52" spans="2:9" x14ac:dyDescent="0.25">
       <c r="E52" s="3"/>
     </row>
-    <row r="55" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="55" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B55" s="1"/>
     </row>
-    <row r="56" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="56" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B56" s="1"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
small bugfix in values (MPNs were right)
</commit_message>
<xml_diff>
--- a/RGB Bypass/BOM_SNES_RGB_bypass.xlsx
+++ b/RGB Bypass/BOM_SNES_RGB_bypass.xlsx
@@ -1514,7 +1514,7 @@
       <c r="C17" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="D17" s="13" t="s">
+      <c r="D17" s="15" t="s">
         <v>15</v>
       </c>
       <c r="E17" t="s">
@@ -1535,7 +1535,7 @@
         <v>46</v>
       </c>
       <c r="C18" s="14"/>
-      <c r="D18" s="13"/>
+      <c r="D18" s="15"/>
       <c r="E18" t="s">
         <v>50</v>
       </c>
@@ -1938,7 +1938,7 @@
         <v>15</v>
       </c>
       <c r="E15" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F15" s="15" t="s">
         <v>14</v>
@@ -1957,7 +1957,7 @@
       <c r="C16" s="16"/>
       <c r="D16" s="15"/>
       <c r="E16" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F16" s="15"/>
       <c r="G16" s="9" t="s">
@@ -2624,7 +2624,7 @@
         <v>15</v>
       </c>
       <c r="E15" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F15" s="15" t="s">
         <v>14</v>
@@ -2643,7 +2643,7 @@
       <c r="C16" s="16"/>
       <c r="D16" s="15"/>
       <c r="E16" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F16" s="15"/>
       <c r="G16" s="9" t="s">

</xml_diff>

<commit_message>
fix some bugs in BOM
</commit_message>
<xml_diff>
--- a/RGB Bypass/BOM_SNES_RGB_bypass.xlsx
+++ b/RGB Bypass/BOM_SNES_RGB_bypass.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10319"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UserData\Bartmann\Documents\Workspaces\Git\SNES-AddOn-PCBs\RGB Bypass\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/ToshibaHDWM110/borti4938/Documents/Workspaces/Git/SNES-AddOn-PCBs/RGB Bypass/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{58E8D655-5012-A140-8A40-BA30882E7873}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="25605" windowHeight="14445"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SNES_RGBAmp" sheetId="1" r:id="rId1"/>
@@ -322,7 +323,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -834,7 +835,7 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
@@ -861,9 +862,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -894,13 +892,13 @@
     <cellStyle name="Akzent6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="Ausgabe" xfId="10" builtinId="21" customBuiltin="1"/>
     <cellStyle name="Berechnung" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="43" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="43" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="44" builtinId="9" hidden="1"/>
     <cellStyle name="Eingabe" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Ergebnis" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Erklärender Text" xfId="16" builtinId="53" customBuiltin="1"/>
     <cellStyle name="Gut" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Link" xfId="42" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="42" builtinId="8"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Notiz" xfId="15" builtinId="10" customBuiltin="1"/>
     <cellStyle name="Schlecht" xfId="7" builtinId="27" customBuiltin="1"/>
@@ -1189,21 +1187,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="16.42578125" customWidth="1"/>
-    <col min="4" max="4" width="23.42578125" customWidth="1"/>
-    <col min="5" max="5" width="18.42578125" customWidth="1"/>
-    <col min="7" max="7" width="59.85546875" customWidth="1"/>
-    <col min="8" max="8" width="11.28515625" customWidth="1"/>
+    <col min="2" max="2" width="16.5" customWidth="1"/>
+    <col min="4" max="4" width="23.5" customWidth="1"/>
+    <col min="5" max="5" width="18.5" customWidth="1"/>
+    <col min="7" max="7" width="59.83203125" customWidth="1"/>
+    <col min="8" max="8" width="11.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -1226,7 +1224,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1245,7 +1243,7 @@
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>18</v>
       </c>
@@ -1261,7 +1259,7 @@
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>23</v>
       </c>
@@ -1277,7 +1275,7 @@
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>24</v>
       </c>
@@ -1293,7 +1291,7 @@
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>28</v>
       </c>
@@ -1315,7 +1313,7 @@
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>29</v>
       </c>
@@ -1337,7 +1335,7 @@
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>73</v>
       </c>
@@ -1356,7 +1354,7 @@
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>53</v>
       </c>
@@ -1381,7 +1379,7 @@
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>32</v>
       </c>
@@ -1403,7 +1401,7 @@
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>35</v>
       </c>
@@ -1425,7 +1423,7 @@
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>36</v>
       </c>
@@ -1450,7 +1448,7 @@
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
         <v>38</v>
       </c>
@@ -1469,11 +1467,11 @@
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>41</v>
       </c>
@@ -1498,18 +1496,18 @@
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C16" s="6"/>
       <c r="G16" s="7"/>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="13" t="s">
         <v>47</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C17" s="14" t="s">
         <v>42</v>
@@ -1518,7 +1516,7 @@
         <v>15</v>
       </c>
       <c r="E17" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F17" s="15" t="s">
         <v>14</v>
@@ -1529,15 +1527,15 @@
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="13"/>
       <c r="B18" s="2" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C18" s="14"/>
       <c r="D18" s="15"/>
       <c r="E18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F18" s="15"/>
       <c r="G18" s="9" t="s">
@@ -1546,19 +1544,19 @@
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" s="12" t="s">
         <v>45</v>
       </c>
@@ -1571,60 +1569,60 @@
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B24" s="2"/>
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B26" s="2"/>
       <c r="E26" s="3"/>
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B27" s="2"/>
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="E28" s="3"/>
       <c r="H28" s="1"/>
       <c r="I28" s="1"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="E30" s="3"/>
       <c r="H30" s="1"/>
       <c r="I30" s="1"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="E31" s="3"/>
       <c r="G31" s="2"/>
       <c r="H31" s="4"/>
       <c r="I31" s="5"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="E32" s="3"/>
       <c r="G32" s="2"/>
       <c r="H32" s="4"/>
       <c r="I32" s="1"/>
     </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B35" s="1"/>
     </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B36" s="1"/>
     </row>
   </sheetData>
@@ -1641,21 +1639,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I48"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="16.42578125" customWidth="1"/>
-    <col min="4" max="4" width="23.42578125" customWidth="1"/>
-    <col min="5" max="5" width="18.42578125" customWidth="1"/>
-    <col min="7" max="7" width="59.85546875" customWidth="1"/>
-    <col min="8" max="8" width="11.28515625" customWidth="1"/>
+    <col min="2" max="2" width="16.5" customWidth="1"/>
+    <col min="4" max="4" width="23.5" customWidth="1"/>
+    <col min="5" max="5" width="18.5" customWidth="1"/>
+    <col min="7" max="7" width="59.83203125" customWidth="1"/>
+    <col min="8" max="8" width="11.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -1678,7 +1676,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1697,7 +1695,7 @@
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>18</v>
       </c>
@@ -1713,7 +1711,7 @@
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>28</v>
       </c>
@@ -1735,7 +1733,7 @@
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>29</v>
       </c>
@@ -1757,7 +1755,7 @@
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>73</v>
       </c>
@@ -1776,7 +1774,7 @@
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>53</v>
       </c>
@@ -1801,7 +1799,7 @@
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>32</v>
       </c>
@@ -1823,7 +1821,7 @@
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>35</v>
       </c>
@@ -1845,7 +1843,7 @@
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>36</v>
       </c>
@@ -1870,7 +1868,7 @@
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
         <v>38</v>
       </c>
@@ -1889,11 +1887,11 @@
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>41</v>
       </c>
@@ -1918,27 +1916,27 @@
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C14" s="6"/>
       <c r="G14" s="7"/>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="13" t="s">
         <v>47</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="C15" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="C15" s="14" t="s">
         <v>42</v>
       </c>
       <c r="D15" s="15" t="s">
         <v>15</v>
       </c>
       <c r="E15" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F15" s="15" t="s">
         <v>14</v>
@@ -1949,15 +1947,15 @@
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="13"/>
       <c r="B16" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="C16" s="16"/>
+        <v>48</v>
+      </c>
+      <c r="C16" s="14"/>
       <c r="D16" s="15"/>
       <c r="E16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F16" s="15"/>
       <c r="G16" s="9" t="s">
@@ -1966,18 +1964,18 @@
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="6" t="s">
         <v>80</v>
       </c>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="s">
         <v>54</v>
       </c>
@@ -1999,7 +1997,7 @@
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="7" t="s">
         <v>57</v>
       </c>
@@ -2021,7 +2019,7 @@
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="7" t="s">
         <v>65</v>
       </c>
@@ -2046,7 +2044,7 @@
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" s="7"/>
       <c r="B22" t="s">
         <v>89</v>
@@ -2069,7 +2067,7 @@
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="7" t="s">
         <v>66</v>
       </c>
@@ -2091,7 +2089,7 @@
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" s="7" t="s">
         <v>69</v>
       </c>
@@ -2116,18 +2114,18 @@
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" s="6" t="s">
         <v>81</v>
       </c>
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" s="7" t="s">
         <v>54</v>
       </c>
@@ -2149,7 +2147,7 @@
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" s="7" t="s">
         <v>57</v>
       </c>
@@ -2171,7 +2169,7 @@
       <c r="H28" s="1"/>
       <c r="I28" s="1"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" s="7" t="s">
         <v>65</v>
       </c>
@@ -2181,7 +2179,7 @@
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" s="7" t="s">
         <v>66</v>
       </c>
@@ -2203,7 +2201,7 @@
       <c r="H30" s="1"/>
       <c r="I30" s="1"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" s="7"/>
       <c r="B31" t="s">
         <v>67</v>
@@ -2214,7 +2212,7 @@
       <c r="H31" s="1"/>
       <c r="I31" s="1"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" s="7" t="s">
         <v>69</v>
       </c>
@@ -2239,12 +2237,12 @@
       <c r="H32" s="1"/>
       <c r="I32" s="1"/>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" s="7"/>
       <c r="H33" s="1"/>
       <c r="I33" s="1"/>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" s="12" t="s">
         <v>45</v>
       </c>
@@ -2257,60 +2255,60 @@
       <c r="H34" s="1"/>
       <c r="I34" s="1"/>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="H35" s="1"/>
       <c r="I35" s="1"/>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B36" s="2"/>
       <c r="H36" s="1"/>
       <c r="I36" s="1"/>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="H37" s="1"/>
       <c r="I37" s="1"/>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B38" s="2"/>
       <c r="E38" s="3"/>
       <c r="H38" s="1"/>
       <c r="I38" s="1"/>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B39" s="2"/>
       <c r="H39" s="1"/>
       <c r="I39" s="1"/>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="E40" s="3"/>
       <c r="H40" s="1"/>
       <c r="I40" s="1"/>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="H41" s="1"/>
       <c r="I41" s="1"/>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="E42" s="3"/>
       <c r="H42" s="1"/>
       <c r="I42" s="1"/>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="E43" s="3"/>
       <c r="G43" s="2"/>
       <c r="H43" s="4"/>
       <c r="I43" s="5"/>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="E44" s="3"/>
       <c r="G44" s="2"/>
       <c r="H44" s="4"/>
       <c r="I44" s="1"/>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B47" s="1"/>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B48" s="1"/>
     </row>
   </sheetData>
@@ -2327,21 +2325,21 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:I56"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="16.42578125" customWidth="1"/>
-    <col min="4" max="4" width="23.42578125" customWidth="1"/>
-    <col min="5" max="5" width="18.42578125" customWidth="1"/>
-    <col min="7" max="7" width="59.85546875" customWidth="1"/>
-    <col min="8" max="8" width="11.28515625" customWidth="1"/>
+    <col min="2" max="2" width="16.5" customWidth="1"/>
+    <col min="4" max="4" width="23.5" customWidth="1"/>
+    <col min="5" max="5" width="18.5" customWidth="1"/>
+    <col min="7" max="7" width="59.83203125" customWidth="1"/>
+    <col min="8" max="8" width="11.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -2364,7 +2362,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -2383,7 +2381,7 @@
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>18</v>
       </c>
@@ -2399,7 +2397,7 @@
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>28</v>
       </c>
@@ -2421,7 +2419,7 @@
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>29</v>
       </c>
@@ -2443,7 +2441,7 @@
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>73</v>
       </c>
@@ -2462,7 +2460,7 @@
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>53</v>
       </c>
@@ -2487,7 +2485,7 @@
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>32</v>
       </c>
@@ -2509,7 +2507,7 @@
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>35</v>
       </c>
@@ -2531,7 +2529,7 @@
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>36</v>
       </c>
@@ -2556,7 +2554,7 @@
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
         <v>38</v>
       </c>
@@ -2575,11 +2573,11 @@
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>41</v>
       </c>
@@ -2604,27 +2602,27 @@
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C14" s="6"/>
       <c r="G14" s="7"/>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="13" t="s">
         <v>47</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="C15" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="C15" s="14" t="s">
         <v>42</v>
       </c>
       <c r="D15" s="15" t="s">
         <v>15</v>
       </c>
       <c r="E15" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F15" s="15" t="s">
         <v>14</v>
@@ -2635,15 +2633,15 @@
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="13"/>
       <c r="B16" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="C16" s="16"/>
+        <v>48</v>
+      </c>
+      <c r="C16" s="14"/>
       <c r="D16" s="15"/>
       <c r="E16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F16" s="15"/>
       <c r="G16" s="9" t="s">
@@ -2652,18 +2650,18 @@
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="6" t="s">
         <v>80</v>
       </c>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="s">
         <v>54</v>
       </c>
@@ -2685,7 +2683,7 @@
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="7" t="s">
         <v>57</v>
       </c>
@@ -2707,7 +2705,7 @@
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="7" t="s">
         <v>65</v>
       </c>
@@ -2732,7 +2730,7 @@
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
         <v>89</v>
       </c>
@@ -2754,7 +2752,7 @@
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="7" t="s">
         <v>66</v>
       </c>
@@ -2773,13 +2771,10 @@
       <c r="F23" t="s">
         <v>14</v>
       </c>
-      <c r="G23" s="7" t="s">
-        <v>43</v>
-      </c>
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" s="7" t="s">
         <v>69</v>
       </c>
@@ -2798,21 +2793,24 @@
       <c r="F24" t="s">
         <v>14</v>
       </c>
+      <c r="G24" s="7" t="s">
+        <v>43</v>
+      </c>
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" s="6" t="s">
         <v>81</v>
       </c>
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" s="7" t="s">
         <v>54</v>
       </c>
@@ -2834,7 +2832,7 @@
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" s="7" t="s">
         <v>57</v>
       </c>
@@ -2853,20 +2851,20 @@
       <c r="F28" t="s">
         <v>14</v>
       </c>
-      <c r="G28" t="s">
-        <v>70</v>
-      </c>
       <c r="H28" s="1"/>
       <c r="I28" s="1"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" s="7" t="s">
         <v>65</v>
       </c>
+      <c r="G29" t="s">
+        <v>70</v>
+      </c>
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" s="7" t="s">
         <v>66</v>
       </c>
@@ -2885,24 +2883,21 @@
       <c r="F30" t="s">
         <v>14</v>
       </c>
-      <c r="G30" t="s">
-        <v>68</v>
-      </c>
       <c r="H30" s="1"/>
       <c r="I30" s="1"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" s="7"/>
       <c r="B31" t="s">
         <v>67</v>
       </c>
-      <c r="G31" s="7" t="s">
-        <v>43</v>
+      <c r="G31" t="s">
+        <v>68</v>
       </c>
       <c r="H31" s="1"/>
       <c r="I31" s="1"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" s="7" t="s">
         <v>69</v>
       </c>
@@ -2921,25 +2916,25 @@
       <c r="F32" t="s">
         <v>14</v>
       </c>
+      <c r="G32" s="7" t="s">
+        <v>43</v>
+      </c>
       <c r="H32" s="1"/>
       <c r="I32" s="1"/>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" s="7"/>
       <c r="H33" s="1"/>
       <c r="I33" s="1"/>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="G34" t="s">
-        <v>87</v>
-      </c>
       <c r="H34" s="1"/>
       <c r="I34" s="1"/>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" s="7" t="s">
         <v>83</v>
       </c>
@@ -2959,12 +2954,12 @@
         <v>14</v>
       </c>
       <c r="G35" t="s">
-        <v>40</v>
+        <v>87</v>
       </c>
       <c r="H35" s="1"/>
       <c r="I35" s="1"/>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" s="6"/>
       <c r="B36" t="s">
         <v>38</v>
@@ -2979,12 +2974,12 @@
         <v>14</v>
       </c>
       <c r="G36" t="s">
-        <v>76</v>
+        <v>40</v>
       </c>
       <c r="H36" s="1"/>
       <c r="I36" s="1"/>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" s="7" t="s">
         <v>84</v>
       </c>
@@ -3004,12 +2999,12 @@
         <v>77</v>
       </c>
       <c r="G37" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="H37" s="1"/>
       <c r="I37" s="1"/>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" s="7"/>
       <c r="B38" t="s">
         <v>71</v>
@@ -3026,10 +3021,13 @@
       <c r="F38" t="s">
         <v>77</v>
       </c>
+      <c r="G38" t="s">
+        <v>88</v>
+      </c>
       <c r="H38" s="1"/>
       <c r="I38" s="1"/>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" s="7" t="s">
         <v>85</v>
       </c>
@@ -3048,13 +3046,10 @@
       <c r="F39" t="s">
         <v>14</v>
       </c>
-      <c r="G39" s="7" t="s">
-        <v>43</v>
-      </c>
       <c r="H39" s="1"/>
       <c r="I39" s="1"/>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" s="7" t="s">
         <v>86</v>
       </c>
@@ -3073,16 +3068,19 @@
       <c r="F40" t="s">
         <v>14</v>
       </c>
+      <c r="G40" s="7" t="s">
+        <v>43</v>
+      </c>
       <c r="H40" s="1"/>
       <c r="I40" s="1"/>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" s="7"/>
       <c r="G41" s="8"/>
       <c r="H41" s="1"/>
       <c r="I41" s="1"/>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" s="8" t="s">
         <v>45</v>
       </c>
@@ -3094,58 +3092,58 @@
       <c r="H42" s="1"/>
       <c r="I42" s="1"/>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="H43" s="1"/>
       <c r="I43" s="1"/>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B44" s="2"/>
       <c r="H44" s="1"/>
       <c r="I44" s="1"/>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="H45" s="1"/>
       <c r="I45" s="1"/>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B46" s="2"/>
       <c r="E46" s="3"/>
       <c r="H46" s="1"/>
       <c r="I46" s="1"/>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B47" s="2"/>
       <c r="H47" s="1"/>
       <c r="I47" s="1"/>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="E48" s="3"/>
       <c r="H48" s="1"/>
       <c r="I48" s="1"/>
     </row>
-    <row r="49" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:9" x14ac:dyDescent="0.2">
       <c r="H49" s="1"/>
       <c r="I49" s="1"/>
     </row>
-    <row r="50" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:9" x14ac:dyDescent="0.2">
       <c r="E50" s="3"/>
       <c r="G50" s="2"/>
       <c r="H50" s="4"/>
       <c r="I50" s="5"/>
     </row>
-    <row r="51" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:9" x14ac:dyDescent="0.2">
       <c r="E51" s="3"/>
       <c r="G51" s="2"/>
       <c r="H51" s="4"/>
       <c r="I51" s="1"/>
     </row>
-    <row r="52" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:9" x14ac:dyDescent="0.2">
       <c r="E52" s="3"/>
     </row>
-    <row r="55" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B55" s="1"/>
     </row>
-    <row r="56" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B56" s="1"/>
     </row>
   </sheetData>

</xml_diff>